<commit_message>
feat(solution): finish export pdf
</commit_message>
<xml_diff>
--- a/docs/public/resources/b2c/solution.xlsx
+++ b/docs/public/resources/b2c/solution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/html/PowerXDocs/docs/public/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/html/PowerXDocs/docs/public/resources/b2c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830AD250-080A-3F4B-9938-855F299B185A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE055D-8B07-9042-A3BB-0C0932198AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23320" yWindow="-20620" windowWidth="26420" windowHeight="18880" xr2:uid="{F3554E28-5F1A-B746-8397-F7310971FB48}"/>
+    <workbookView xWindow="-20380" yWindow="-21100" windowWidth="26420" windowHeight="18880" activeTab="2" xr2:uid="{F3554E28-5F1A-B746-8397-F7310971FB48}"/>
   </bookViews>
   <sheets>
     <sheet name="干系人" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>项目</t>
   </si>
@@ -47,18 +47,6 @@
   </si>
   <si>
     <t>系统使用者</t>
-  </si>
-  <si>
-    <t>品牌的组织架构人员，品牌分销渠道</t>
-  </si>
-  <si>
-    <t>品牌合作伙伴</t>
-  </si>
-  <si>
-    <t>第三方相关者</t>
-  </si>
-  <si>
-    <t>经销商</t>
   </si>
   <si>
     <t>负责CRM的核心业务流程，跟进客户的商业生命周期</t>
@@ -88,24 +76,9 @@
     <t>第三方电商平台</t>
   </si>
   <si>
-    <t>品牌分销渠道</t>
-  </si>
-  <si>
     <t>定期的优惠活动和事件，可以帮助品牌的营销团队制定活动策划和大促活动</t>
   </si>
   <si>
-    <t>负责各自大区域市场的销售体系
-配合品牌方一起做相应的市场活动
-管理下级子代理的各种销售活动
-负责供货给下级分销商</t>
-  </si>
-  <si>
-    <t>微商</t>
-  </si>
-  <si>
-    <t>负责从代理商拿货，供给终端客户</t>
-  </si>
-  <si>
     <t>第三方支付监管</t>
   </si>
   <si>
@@ -125,9 +98,6 @@
   </si>
   <si>
     <t>市场策划主管</t>
-  </si>
-  <si>
-    <t>协助制定销售计划</t>
   </si>
   <si>
     <t xml:space="preserve">根据不同类型的目标，来衡量
@@ -215,13 +185,6 @@
 提供最优的IT解决方案</t>
   </si>
   <si>
-    <t>华东区总代理</t>
-  </si>
-  <si>
-    <t>完成和品牌达成的年销售额目标
-保证品牌的市场价值</t>
-  </si>
-  <si>
     <t>协助系统集成的API</t>
   </si>
   <si>
@@ -263,33 +226,7 @@
 可以有金融分期支付功能</t>
   </si>
   <si>
-    <t>门店</t>
-  </si>
-  <si>
-    <t>可以自行注册门店账号，挂靠在一级或者二级代理商下
-可以提供门店的地理位置，让客户可以通过LBS推荐或搜索到
-随时可以移动端登陆，做相关业务操作</t>
-  </si>
-  <si>
     <t>小程序/APP/Web</t>
-  </si>
-  <si>
-    <t>品牌多层代理</t>
-  </si>
-  <si>
-    <t>系统可以提供自动分账功能
-系统可以提供门店或经销商关联挂靠</t>
-  </si>
-  <si>
-    <t>负责从品牌拿货，供给终端客户</t>
-  </si>
-  <si>
-    <t>希望系统提供一件代发的功能，不用自己囤货
-只能发出确认的授权区域内授权订单</t>
-  </si>
-  <si>
-    <t>可以自行注册门店账号，挂靠在一级或者二级代理商下
-随时可以移动端登陆，做相关业务操作</t>
   </si>
   <si>
     <t>可以在系统上架商品信息
@@ -344,6 +281,9 @@
   </si>
   <si>
     <t>干系人的期望</t>
+  </si>
+  <si>
+    <t>品牌的组织架构人员</t>
   </si>
 </sst>
 </file>
@@ -542,8 +482,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CBA6D5-349B-F148-B32A-1F13483C1585}" name="Table2" displayName="Table2" ref="A1:B15" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
-  <autoFilter ref="A1:B15" xr:uid="{E0CBA6D5-349B-F148-B32A-1F13483C1585}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0CBA6D5-349B-F148-B32A-1F13483C1585}" name="Table2" displayName="Table2" ref="A1:B11" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
+  <autoFilter ref="A1:B11" xr:uid="{E0CBA6D5-349B-F148-B32A-1F13483C1585}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CD5A26EE-20C6-4447-AECE-FCBBF1BB4A98}" name="干系人" dataDxfId="5" dataCellStyle="tb_cell"/>
     <tableColumn id="2" xr3:uid="{C1523F9C-4ED0-7641-8ECD-769A99A42EBC}" name="干系人工作职责" dataCellStyle="tb_cell"/>
@@ -553,8 +493,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3450F6AA-7E7C-EC4E-A7EB-7E1EF1151116}" name="Table3" displayName="Table3" ref="A18:B22" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
-  <autoFilter ref="A18:B22" xr:uid="{3450F6AA-7E7C-EC4E-A7EB-7E1EF1151116}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3450F6AA-7E7C-EC4E-A7EB-7E1EF1151116}" name="Table3" displayName="Table3" ref="A14:B18" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
+  <autoFilter ref="A14:B18" xr:uid="{3450F6AA-7E7C-EC4E-A7EB-7E1EF1151116}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{AD0332E9-9577-7048-A53B-8706166F7D20}" name="干系人" dataDxfId="4" dataCellStyle="tb_cell"/>
     <tableColumn id="2" xr3:uid="{7C286C02-2087-4E42-B4E7-B4FDD46E6C23}" name="市场人员" dataCellStyle="tb_cell"/>
@@ -564,8 +504,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85AD6198-4621-2749-A774-DAB4AF59B785}" name="Table35" displayName="Table35" ref="A25:B29" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
-  <autoFilter ref="A25:B29" xr:uid="{85AD6198-4621-2749-A774-DAB4AF59B785}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85AD6198-4621-2749-A774-DAB4AF59B785}" name="Table35" displayName="Table35" ref="A21:B25" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
+  <autoFilter ref="A21:B25" xr:uid="{85AD6198-4621-2749-A774-DAB4AF59B785}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4F3136E0-0F1F-C14B-BD44-565F2786CD52}" name="干系人" dataDxfId="3" dataCellStyle="tb_cell"/>
     <tableColumn id="2" xr3:uid="{841CB228-E471-834E-9988-DCB163CC4A74}" name="运营人员" dataCellStyle="tb_cell"/>
@@ -575,8 +515,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{593480EE-B755-6C4E-A436-E479B810002E}" name="Table357" displayName="Table357" ref="A32:B36" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
-  <autoFilter ref="A32:B36" xr:uid="{593480EE-B755-6C4E-A436-E479B810002E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{593480EE-B755-6C4E-A436-E479B810002E}" name="Table357" displayName="Table357" ref="A28:B32" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
+  <autoFilter ref="A28:B32" xr:uid="{593480EE-B755-6C4E-A436-E479B810002E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8DA3BA20-70D0-2443-BD4C-1E00A18106E2}" name="干系人" dataDxfId="2" dataCellStyle="tb_cell"/>
     <tableColumn id="2" xr3:uid="{BB76F485-5D86-9546-BA29-E9995DD55B58}" name="销售人员" dataCellStyle="tb_cell"/>
@@ -586,8 +526,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{093F3481-9D7A-CE47-8A58-0F3D1B7A6D8E}" name="Table5" displayName="Table5" ref="A1:D23" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
-  <autoFilter ref="A1:D23" xr:uid="{093F3481-9D7A-CE47-8A58-0F3D1B7A6D8E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{093F3481-9D7A-CE47-8A58-0F3D1B7A6D8E}" name="Table5" displayName="Table5" ref="A1:D9" totalsRowShown="0" headerRowCellStyle="tb_head" dataCellStyle="tb_cell">
+  <autoFilter ref="A1:D9" xr:uid="{093F3481-9D7A-CE47-8A58-0F3D1B7A6D8E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{94485D24-39B5-4241-AB41-F6A6D77BB789}" name="干系人名称" dataDxfId="1" dataCellStyle="tb_cell"/>
     <tableColumn id="2" xr3:uid="{593E9FD4-8095-244B-B4A7-EC9264E8CC52}" name="工作职责和特点" dataCellStyle="tb_cell"/>
@@ -900,9 +840,9 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -932,16 +872,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -954,9 +890,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9355D976-DC1E-914A-87C1-BE0CE75589C8}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="143" zoomScaleNormal="143" zoomScaleSheetLayoutView="107" workbookViewId="0"/>
+    <sheetView zoomScale="143" zoomScaleNormal="143" zoomScaleSheetLayoutView="107" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -966,424 +904,372 @@
     <col min="8" max="8" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="128" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>53</v>
+    </row>
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="A25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="G28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="G29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="G30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+      <c r="G31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="G32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1400,9 +1286,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBDAD88-88C8-004D-8D2E-273902907404}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1414,16 +1302,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -1431,213 +1319,99 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>18</v>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>